<commit_message>
Social-Security & AdHoc Dependents Modify
</commit_message>
<xml_diff>
--- a/MLSD-BOM/resources/DynamicDomains.xlsx
+++ b/MLSD-BOM/resources/DynamicDomains.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2831" uniqueCount="2501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2851" uniqueCount="2519">
   <si>
     <t>Values</t>
   </si>
@@ -7536,6 +7536,60 @@
   </si>
   <si>
     <t>اسقاط المستفيد بسبب عدم وجود فئة استحقاق</t>
+  </si>
+  <si>
+    <t>MSGDE15</t>
+  </si>
+  <si>
+    <t>Invalid Dependent Is Married Or Has Offsprings</t>
+  </si>
+  <si>
+    <t>MSG-DE15</t>
+  </si>
+  <si>
+    <t>اسقاط التابع بسبب أنه متزوج أو له أولاد</t>
+  </si>
+  <si>
+    <t>MSGDE16</t>
+  </si>
+  <si>
+    <t>MSG-DE16</t>
+  </si>
+  <si>
+    <t>Invalid Dependent Is Not A Student</t>
+  </si>
+  <si>
+    <t>اسقاط التابع بسبب انه ليس طالب</t>
+  </si>
+  <si>
+    <t>MSGDE17</t>
+  </si>
+  <si>
+    <t>MSG-DE17</t>
+  </si>
+  <si>
+    <t>MSGDE18</t>
+  </si>
+  <si>
+    <t>Invalid Dependent Marital Status Check</t>
+  </si>
+  <si>
+    <t>MSG-DE18</t>
+  </si>
+  <si>
+    <t>اسقاط التابع بسبب عدم توافق الحالة الاجتماعية</t>
+  </si>
+  <si>
+    <t>MSGCD3</t>
+  </si>
+  <si>
+    <t>MSG-CD3</t>
+  </si>
+  <si>
+    <t>Invalid Dependent is Blacklisted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اسقاط التابع بسبب ادراجه ضمن القائمة المحظورة </t>
   </si>
 </sst>
 </file>
@@ -12225,10 +12279,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E179" sqref="E179"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D186" sqref="D186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15311,7 +15365,7 @@
         <v>2465</v>
       </c>
       <c r="D171" s="6" t="str">
-        <f t="shared" ref="D171:D179" si="10">CONCATENATE("return new RejectionMessageDetails(""",C171,"""",",""",B171,"""",",""",E171,""")",";")</f>
+        <f t="shared" ref="D171:D180" si="10">CONCATENATE("return new RejectionMessageDetails(""",C171,"""",",""",B171,"""",",""",E171,""")",";")</f>
         <v>return new RejectionMessageDetails("MSG-ML14","Invalid Applicant Is Not DSS Eligible And Applying For Inclusive Support","اسقاط المستفيد بسبب انه غير مسجل في برنامج معاش الضمان الأجتماعي و مقدم في المساعدة مشمولة");</v>
       </c>
       <c r="E171" s="13" t="s">
@@ -15460,6 +15514,96 @@
       </c>
       <c r="E179" s="10" t="s">
         <v>2500</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="4" t="s">
+        <v>2501</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>2502</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>2503</v>
+      </c>
+      <c r="D180" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>return new RejectionMessageDetails("MSG-DE15","Invalid Dependent Is Married Or Has Offsprings","اسقاط التابع بسبب أنه متزوج أو له أولاد");</v>
+      </c>
+      <c r="E180" s="10" t="s">
+        <v>2504</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="4" t="s">
+        <v>2505</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>2507</v>
+      </c>
+      <c r="C181" s="4" t="s">
+        <v>2506</v>
+      </c>
+      <c r="D181" s="4" t="str">
+        <f t="shared" ref="D181" si="11">CONCATENATE("return new RejectionMessageDetails(""",C181,"""",",""",B181,"""",",""",E181,""")",";")</f>
+        <v>return new RejectionMessageDetails("MSG-DE16","Invalid Dependent Is Not A Student","اسقاط التابع بسبب انه ليس طالب");</v>
+      </c>
+      <c r="E181" s="10" t="s">
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="4" t="s">
+        <v>2509</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="C182" s="4" t="s">
+        <v>2510</v>
+      </c>
+      <c r="D182" s="4" t="str">
+        <f t="shared" ref="D182:D184" si="12">CONCATENATE("return new RejectionMessageDetails(""",C182,"""",",""",B182,"""",",""",E182,""")",";")</f>
+        <v>return new RejectionMessageDetails("MSG-DE17","Invalid Dependent Age Check","اسقاط التابع بسبب عدم توافق العمر مع الضوابط ");</v>
+      </c>
+      <c r="E182" s="10" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="4" t="s">
+        <v>2511</v>
+      </c>
+      <c r="B183" s="4" t="s">
+        <v>2512</v>
+      </c>
+      <c r="C183" s="4" t="s">
+        <v>2513</v>
+      </c>
+      <c r="D183" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>return new RejectionMessageDetails("MSG-DE18","Invalid Dependent Marital Status Check","اسقاط التابع بسبب عدم توافق الحالة الاجتماعية");</v>
+      </c>
+      <c r="E183" s="10" t="s">
+        <v>2514</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="4" t="s">
+        <v>2515</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>2517</v>
+      </c>
+      <c r="C184" s="4" t="s">
+        <v>2516</v>
+      </c>
+      <c r="D184" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>return new RejectionMessageDetails("MSG-CD3","Invalid Dependent is Blacklisted","اسقاط التابع بسبب ادراجه ضمن القائمة المحظورة ");</v>
+      </c>
+      <c r="E184" s="5" t="s">
+        <v>2518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Medical Equipment Service CR
</commit_message>
<xml_diff>
--- a/MLSD-BOM/resources/DynamicDomains.xlsx
+++ b/MLSD-BOM/resources/DynamicDomains.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2879" uniqueCount="2543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2887" uniqueCount="2551">
   <si>
     <t>Values</t>
   </si>
@@ -7662,6 +7662,30 @@
   </si>
   <si>
     <t>عزرا، تم تجاوز عدد الاجهزه الطبية في الطلب</t>
+  </si>
+  <si>
+    <t>MSGME8</t>
+  </si>
+  <si>
+    <t>Invalid Applicant Disability Does Not Support This Service</t>
+  </si>
+  <si>
+    <t>MSG-ME8</t>
+  </si>
+  <si>
+    <t>عذرا، لا يمكنك تقديم طلب ويجب عمل تحديث لبيانات الاعاقة (لا يوجد اعاقة تتيح هذه الخدمة) للمستفيد</t>
+  </si>
+  <si>
+    <t>MSGME9</t>
+  </si>
+  <si>
+    <t>Invalid Applicant Has Similar Equipments In The Request</t>
+  </si>
+  <si>
+    <t>MSG-ME9</t>
+  </si>
+  <si>
+    <t>عذرا، لا يمكنك تقديم الطلب بسبب تكرار احد الاجهزة في الطلب</t>
   </si>
 </sst>
 </file>
@@ -12353,10 +12377,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E191"/>
+  <dimension ref="A1:E193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D193" sqref="D193"/>
+    <sheetView tabSelected="1" topLeftCell="A177" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D195" sqref="D195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15802,8 +15826,44 @@
         <f t="shared" si="12"/>
         <v>return new RejectionMessageDetails("MSG-ME7","Invalid Applicant Exceeded The Number Of Medical Equipments In The Request","عزرا، تم تجاوز عدد الاجهزه الطبية في الطلب");</v>
       </c>
-      <c r="E191" s="6" t="s">
+      <c r="E191" s="11" t="s">
         <v>2542</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A192" s="6" t="s">
+        <v>2543</v>
+      </c>
+      <c r="B192" s="6" t="s">
+        <v>2544</v>
+      </c>
+      <c r="C192" s="6" t="s">
+        <v>2545</v>
+      </c>
+      <c r="D192" s="6" t="str">
+        <f t="shared" ref="D192:D193" si="13">CONCATENATE("return new RejectionMessageDetails(""",C192,"""",",""",B192,"""",",""",E192,""")",";")</f>
+        <v>return new RejectionMessageDetails("MSG-ME8","Invalid Applicant Disability Does Not Support This Service","عذرا، لا يمكنك تقديم طلب ويجب عمل تحديث لبيانات الاعاقة (لا يوجد اعاقة تتيح هذه الخدمة) للمستفيد");</v>
+      </c>
+      <c r="E192" s="12" t="s">
+        <v>2546</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="6" t="s">
+        <v>2547</v>
+      </c>
+      <c r="B193" s="6" t="s">
+        <v>2548</v>
+      </c>
+      <c r="C193" s="6" t="s">
+        <v>2549</v>
+      </c>
+      <c r="D193" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>return new RejectionMessageDetails("MSG-ME9","Invalid Applicant Has Similar Equipments In The Request","عذرا، لا يمكنك تقديم الطلب بسبب تكرار احد الاجهزة في الطلب");</v>
+      </c>
+      <c r="E193" s="11" t="s">
+        <v>2550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>